<commit_message>
fin journée 22.04.24, création du projet sur Visual Studio
</commit_message>
<xml_diff>
--- a/Journal-de-Travail_ZeqiriAmir.xlsx
+++ b/Journal-de-Travail_ZeqiriAmir.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps70dji\Desktop\GitHub\P_App-335\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9402146-AC3D-4E4B-80E6-E66E6AE78BDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD8B235-3734-4B06-9B56-F94C4DB55702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="Mvap2W10CJFFJsnvkGXSiMLvpngxTMJbJsIKFe7Hzjn0XDcmjGuvBC2FjUCZ/hpRpUhUrG1T4kBlDAIo3yqmSQ==" workbookSaltValue="KXjgXOcsUZI/j7UgPKltzw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Journal de travail</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>Finalisation de la maquette</t>
+  </si>
+  <si>
+    <t>Création du projet sur Visual Studio</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1066,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.10069444444444445</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1994,7 +1997,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2047,7 +2050,7 @@
       </c>
       <c r="C3" s="23" t="str">
         <f>INT(E4/1440)&amp;" jours "&amp;INT(MOD(E4/1440,1)*24)&amp;" heurs "&amp;INT(MOD(MOD(E4/1440,1)*24,1)*60)&amp;" minutes"</f>
-        <v>0 jours 6 heurs 40 minutes</v>
+        <v>0 jours 9 heurs 4 minutes</v>
       </c>
       <c r="D3" s="23"/>
       <c r="E3" s="3"/>
@@ -2062,15 +2065,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="23">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>300</v>
+        <v>420</v>
       </c>
       <c r="D4" s="23">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>100</v>
+        <v>125</v>
       </c>
       <c r="E4" s="41">
         <f>SUM(C4:D4)</f>
-        <v>400</v>
+        <v>545</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="7"/>
@@ -2247,15 +2250,25 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="str">
+      <c r="A12" s="8">
         <f>IF(ISBLANK(B12),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B12))</f>
-        <v/>
-      </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="50"/>
-      <c r="F12" s="37"/>
+        <v>17</v>
+      </c>
+      <c r="B12" s="47">
+        <v>45404</v>
+      </c>
+      <c r="C12" s="48">
+        <v>2</v>
+      </c>
+      <c r="D12" s="49">
+        <v>25</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="37" t="s">
+        <v>34</v>
+      </c>
       <c r="G12" s="16"/>
       <c r="M12" t="s">
         <v>7</v>
@@ -8649,11 +8662,11 @@
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$C$7:$C$532)*60</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="B5">
         <f>SUMIF('Journal de travail'!$E$7:$E$532,Analyse!C5,'Journal de travail'!$D$7:$D$532)</f>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="C5" s="42" t="str">
         <f>'Journal de travail'!M9</f>
@@ -8661,7 +8674,7 @@
       </c>
       <c r="D5" s="34">
         <f t="shared" ref="D5:D11" si="0">(A5+B5)/1440</f>
-        <v>0</v>
+        <v>0.10069444444444445</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
@@ -8770,7 +8783,7 @@
       </c>
       <c r="D12" s="35">
         <f>SUM(D4:D11)</f>
-        <v>6.9444444444444448E-2</v>
+        <v>0.1701388888888889</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -8795,15 +8808,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D4F20F00DBE2EE49BE9523363A2DF18B" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="313dbdbec26224d1c2bb7e3c488b2a4e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="99ffe1f3-7857-457f-add0-5bdef636f38d" xmlns:ns3="be0d3259-a7ce-4623-88ec-81594dfcbc1c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4739345e3d2c6be79c5ae1a54d02a4a7" ns2:_="" ns3:_="">
     <xsd:import namespace="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
@@ -9026,6 +9030,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
@@ -9038,14 +9051,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F2FB702A-DCBD-43A8-A34C-6000FD8861AD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9062,4 +9067,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>